<commit_message>
Mise à jour des données des cartes
</commit_message>
<xml_diff>
--- a/Splendor_Cartes - sans requetes.xlsx
+++ b/Splendor_Cartes - sans requetes.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projet\SplendorGameJoaoCyril\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0013A584-17D3-4609-A485-F5A73F5899C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -53,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -380,11 +386,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
@@ -399,8 +405,8 @@
     <col min="7" max="7" width="6.42578125" customWidth="1"/>
     <col min="8" max="8" width="6.28515625" customWidth="1"/>
     <col min="9" max="9" width="7.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
     <col min="12" max="12" width="10.42578125" customWidth="1"/>
     <col min="13" max="13" width="11.28515625" customWidth="1"/>
     <col min="14" max="14" width="17.5703125" customWidth="1"/>
@@ -451,23 +457,23 @@
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (2, 0,4,3)</v>
       </c>
       <c r="J2" t="str">
-        <f>IF(NOT(ISBLANK(D2)),"insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(D2)-3&amp;","&amp;D2&amp;")","")</f>
+        <f t="shared" ref="J2:J65" si="0">IF(NOT(ISBLANK(D2)),"sql = ""insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(D2)-4&amp;","&amp;D2&amp;")""; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();","")</f>
         <v/>
       </c>
       <c r="K2" t="str">
-        <f>IF(NOT(ISBLANK(E2)),"insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(E2)-3&amp;","&amp;E2&amp;")","")</f>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (2, 2,4)</v>
+        <f t="shared" ref="K2:K65" si="1">IF(NOT(ISBLANK(E2)),"sql = ""insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(E2)-4&amp;","&amp;E2&amp;")""; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();","")</f>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (2, 1,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L2" t="str">
-        <f>IF(NOT(ISBLANK(F2)),"insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(F2)-3&amp;","&amp;F2&amp;")","")</f>
+        <f t="shared" ref="L2:L65" si="2">IF(NOT(ISBLANK(F2)),"sql = ""insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(F2)-4&amp;","&amp;F2&amp;")""; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();","")</f>
         <v/>
       </c>
       <c r="M2" t="str">
-        <f>IF(NOT(ISBLANK(G2)),"insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(G2)-3&amp;","&amp;G2&amp;")","")</f>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (2, 4,4)</v>
+        <f t="shared" ref="M2:M65" si="3">IF(NOT(ISBLANK(G2)),"sql = ""insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(G2)-4&amp;","&amp;G2&amp;")""; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();","")</f>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (2, 3,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N2" t="str">
-        <f>IF(NOT(ISBLANK(H2)),"insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(H2)-3&amp;","&amp;H2&amp;")","")</f>
+        <f t="shared" ref="N2:N65" si="4">IF(NOT(ISBLANK(H2)),"sql = ""insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(H2)-4&amp;","&amp;H2&amp;")""; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();","")</f>
         <v/>
       </c>
     </row>
@@ -489,23 +495,23 @@
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (3, 0,4,3)</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J66" si="0">IF(NOT(ISBLANK(D3)),"insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(D3)-3&amp;","&amp;D3&amp;")","")</f>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (3, 1,4)</v>
+        <f t="shared" si="0"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (3, 0,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K66" si="1">IF(NOT(ISBLANK(E3)),"insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(E3)-3&amp;","&amp;E3&amp;")","")</f>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (3, 2,4)</v>
+        <f t="shared" si="1"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (3, 1,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:M66" si="2">IF(NOT(ISBLANK(F3)),"insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(F3)-3&amp;","&amp;F3&amp;")","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N66" si="3">IF(NOT(ISBLANK(H3)),"insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(H3)-3&amp;","&amp;H3&amp;")","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -526,7 +532,7 @@
         <v>3</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I11" si="4">"insert into card(idcard, fkRessource, level, nbPtPrestige) values ("&amp;ROW()&amp;", 0,"&amp;A4&amp;","&amp;C4&amp;")"</f>
+        <f t="shared" ref="I4:I11" si="5">"insert into card(idcard, fkRessource, level, nbPtPrestige) values ("&amp;ROW()&amp;", 0,"&amp;A4&amp;","&amp;C4&amp;")"</f>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (4, 0,4,3)</v>
       </c>
       <c r="J4" t="str">
@@ -539,15 +545,15 @@
       </c>
       <c r="L4" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (4, 3,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (4, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (4, 4,3)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (4, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (4, 5,3)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (4, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -564,7 +570,7 @@
         <v>4</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (5, 0,4,3)</v>
       </c>
       <c r="J5" t="str">
@@ -577,15 +583,15 @@
       </c>
       <c r="L5" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (5, 3,4)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (5, 2,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N5" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (5, 5,4)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (5, 4,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -602,12 +608,12 @@
         <v>4</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (6, 0,4,3)</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (6, 1,4)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (6, 0,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
@@ -615,14 +621,14 @@
       </c>
       <c r="L6" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (6, 3,4)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (6, 2,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -643,12 +649,12 @@
         <v>3</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (7, 0,4,3)</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (7, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (7, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="1"/>
@@ -656,15 +662,15 @@
       </c>
       <c r="L7" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (7, 3,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (7, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (7, 5,3)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (7, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -684,7 +690,7 @@
         <v>3</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (8, 0,4,3)</v>
       </c>
       <c r="J8" t="str">
@@ -693,19 +699,19 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (8, 2,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (8, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (8, 4,3)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (8, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (8, 5,3)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (8, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -725,27 +731,27 @@
         <v>3</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (9, 0,4,3)</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (9, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (9, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (9, 2,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (9, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (9, 4,3)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (9, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -763,7 +769,7 @@
         <v>4</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (10, 0,4,3)</v>
       </c>
       <c r="J10" t="str">
@@ -779,12 +785,12 @@
         <v/>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (10, 4,4)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (10, 3,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (10, 5,4)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (10, 4,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -804,27 +810,27 @@
         <v>3</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (11, 0,4,3)</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (11, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (11, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (11, 2,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (11, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (11, 3,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (11, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -861,12 +867,12 @@
         <v/>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (12, 4,3)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (12, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (12, 5,7)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (12, 4,7)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -886,12 +892,12 @@
         <v>3</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" ref="I13:I76" si="5">"insert into card(idcard, fkRessource, level, nbPtPrestige) values (" &amp; ROW() &amp;"," &amp; B13 &amp; "," &amp; A13 &amp; "," &amp; C13 &amp; ")"</f>
+        <f t="shared" ref="I13:I76" si="6">"insert into card(idcard, fkRessource, level, nbPtPrestige) values (" &amp; ROW() &amp;"," &amp; B13 &amp; "," &amp; A13 &amp; "," &amp; C13 &amp; ")"</f>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (13,3,3,5)</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (13, 1,7)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (13, 0,7)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="1"/>
@@ -899,14 +905,14 @@
       </c>
       <c r="L13" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (13, 3,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (13, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -933,12 +939,12 @@
         <v>5</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (14,2,3,3)</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (14, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (14, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="1"/>
@@ -946,15 +952,15 @@
       </c>
       <c r="L14" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (14, 3,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (14, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (14, 4,3)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (14, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (14, 5,5)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (14, 4,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -980,27 +986,27 @@
         <v>3</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (15,5,3,3)</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (15, 1,5)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (15, 0,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (15, 2,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (15, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (15, 3,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (15, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (15, 4,3)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (15, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1024,27 +1030,27 @@
         <v>3</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (16,1,3,4)</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (16, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (16, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (16, 2,6)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (16, 1,6)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (16, 4,3)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (16, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1077,19 +1083,19 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (17, 2,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (17, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M17" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (17, 4,6)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (17, 3,6)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N17" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (17, 5,3)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (17, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -1106,7 +1112,7 @@
         <v>7</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (18,5,3,4)</v>
       </c>
       <c r="J18" t="str">
@@ -1119,14 +1125,14 @@
       </c>
       <c r="L18" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (18, 3,7)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (18, 2,7)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1147,7 +1153,7 @@
         <v>3</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (19,5,3,5)</v>
       </c>
       <c r="J19" t="str">
@@ -1160,15 +1166,15 @@
       </c>
       <c r="L19" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (19, 3,7)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (19, 2,7)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N19" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (19, 5,3)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (19, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -1185,7 +1191,7 @@
         <v>7</v>
       </c>
       <c r="I20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (20,1,3,4)</v>
       </c>
       <c r="J20" t="str">
@@ -1194,18 +1200,18 @@
       </c>
       <c r="K20" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (20, 2,7)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (20, 1,7)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1229,7 +1235,7 @@
         <v>6</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (21,4,3,4)</v>
       </c>
       <c r="J21" t="str">
@@ -1242,15 +1248,15 @@
       </c>
       <c r="L21" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (21, 3,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (21, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M21" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (21, 4,3)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (21, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N21" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (21, 5,6)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (21, 4,6)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -1270,7 +1276,7 @@
         <v>7</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (22,2,3,5)</v>
       </c>
       <c r="J22" t="str">
@@ -1279,18 +1285,18 @@
       </c>
       <c r="K22" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (22, 2,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (22, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M22" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (22, 4,7)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (22, 3,7)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1308,12 +1314,12 @@
         <v>7</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (23,3,3,4)</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (23, 1,7)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (23, 0,7)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="1"/>
@@ -1324,11 +1330,11 @@
         <v/>
       </c>
       <c r="M23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1355,7 +1361,7 @@
         <v>3</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (24,1,3,3)</v>
       </c>
       <c r="J24" t="str">
@@ -1364,19 +1370,19 @@
       </c>
       <c r="K24" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (24, 2,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (24, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (24, 3,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (24, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M24" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (24, 4,5)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (24, 3,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N24" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (24, 5,3)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (24, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -1402,28 +1408,28 @@
         <v>3</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (25,4,3,3)</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (25, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (25, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (25, 2,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (25, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (25, 3,5)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (25, 2,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N25" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (25, 5,3)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (25, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -1440,7 +1446,7 @@
         <v>7</v>
       </c>
       <c r="I26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (26,2,3,4)</v>
       </c>
       <c r="J26" t="str">
@@ -1456,11 +1462,11 @@
         <v/>
       </c>
       <c r="M26" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (26, 4,7)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (26, 3,7)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1484,27 +1490,27 @@
         <v>3</v>
       </c>
       <c r="I27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (27,3,3,4)</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (27, 1,6)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (27, 0,6)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (27, 2,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (27, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (27, 3,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (27, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1522,7 +1528,7 @@
         <v>7</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (28,4,3,4)</v>
       </c>
       <c r="J28" t="str">
@@ -1538,12 +1544,12 @@
         <v/>
       </c>
       <c r="M28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N28" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (28, 5,7)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (28, 4,7)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -1563,27 +1569,27 @@
         <v>7</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (29,1,3,5)</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (29, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (29, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (29, 2,7)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (29, 1,7)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1607,12 +1613,12 @@
         <v>3</v>
       </c>
       <c r="I30" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (30,5,3,4)</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (30, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (30, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K30" t="str">
         <f t="shared" si="1"/>
@@ -1620,15 +1626,15 @@
       </c>
       <c r="L30" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (30, 3,6)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (30, 2,6)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N30" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (30, 5,3)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (30, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
@@ -1654,28 +1660,28 @@
         <v>3</v>
       </c>
       <c r="I31" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (31,3,3,3)</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (31, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (31, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K31" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (31, 2,5)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (31, 1,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M31" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (31, 4,3)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (31, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N31" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (31, 5,3)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (31, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -1692,12 +1698,12 @@
         <v>5</v>
       </c>
       <c r="I32" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (32,5,2,2)</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (32, 1,5)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (32, 0,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K32" t="str">
         <f t="shared" si="1"/>
@@ -1708,11 +1714,11 @@
         <v/>
       </c>
       <c r="M32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1736,12 +1742,12 @@
         <v>3</v>
       </c>
       <c r="I33" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (33,1,2,1)</v>
       </c>
       <c r="J33" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (33, 1,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (33, 0,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K33" t="str">
         <f t="shared" si="1"/>
@@ -1749,14 +1755,14 @@
       </c>
       <c r="L33" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (33, 3,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (33, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M33" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (33, 4,3)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (33, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1780,27 +1786,27 @@
         <v>2</v>
       </c>
       <c r="I34" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (34,5,2,1)</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (34, 1,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (34, 0,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K34" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (34, 2,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (34, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (34, 3,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (34, 2,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1824,27 +1830,27 @@
         <v>2</v>
       </c>
       <c r="I35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (35,5,2,2)</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (35, 1,4)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (35, 0,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K35" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (35, 2,1)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (35, 1,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (35, 3,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (35, 2,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1868,12 +1874,12 @@
         <v>2</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (36,5,2,1)</v>
       </c>
       <c r="J36" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (36, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (36, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K36" t="str">
         <f t="shared" si="1"/>
@@ -1884,12 +1890,12 @@
         <v/>
       </c>
       <c r="M36" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (36, 4,3)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (36, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N36" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (36, 5,2)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (36, 4,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
@@ -1909,7 +1915,7 @@
         <v>5</v>
       </c>
       <c r="I37" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (37,2,2,2)</v>
       </c>
       <c r="J37" t="str">
@@ -1918,18 +1924,18 @@
       </c>
       <c r="K37" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (37, 2,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (37, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M37" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (37, 4,5)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (37, 3,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1953,12 +1959,12 @@
         <v>2</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (38,4,2,2)</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (38, 1,1)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (38, 0,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K38" t="str">
         <f t="shared" si="1"/>
@@ -1966,15 +1972,15 @@
       </c>
       <c r="L38" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (38, 3,4)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (38, 2,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N38" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (38, 5,2)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (38, 4,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
@@ -1997,27 +2003,27 @@
         <v>2</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (39,4,2,1)</v>
       </c>
       <c r="J39" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (39, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (39, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K39" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (39, 2,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (39, 1,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L39" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M39" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (39, 4,2)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (39, 3,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2041,7 +2047,7 @@
         <v>4</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (40,2,2,2)</v>
       </c>
       <c r="J40" t="str">
@@ -2054,15 +2060,15 @@
       </c>
       <c r="L40" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (40, 3,1)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (40, 2,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M40" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (40, 4,2)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (40, 3,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N40" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (40, 5,4)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (40, 4,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
@@ -2079,7 +2085,7 @@
         <v>5</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (41,2,2,2)</v>
       </c>
       <c r="J41" t="str">
@@ -2088,18 +2094,18 @@
       </c>
       <c r="K41" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (41, 2,5)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (41, 1,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L41" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2120,27 +2126,27 @@
         <v>5</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (42,3,2,2)</v>
       </c>
       <c r="J42" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (42, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (42, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K42" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (42, 2,5)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (42, 1,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L42" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2161,7 +2167,7 @@
         <v>3</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (43,1,2,2)</v>
       </c>
       <c r="J43" t="str">
@@ -2174,15 +2180,15 @@
       </c>
       <c r="L43" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (43, 3,5)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (43, 2,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N43" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (43, 5,3)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (43, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
@@ -2199,7 +2205,7 @@
         <v>6</v>
       </c>
       <c r="I44" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (44,5,2,3)</v>
       </c>
       <c r="J44" t="str">
@@ -2215,12 +2221,12 @@
         <v/>
       </c>
       <c r="M44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N44" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (44, 5,6)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (44, 4,6)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
@@ -2237,7 +2243,7 @@
         <v>6</v>
       </c>
       <c r="I45" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (45,4,2,3)</v>
       </c>
       <c r="J45" t="str">
@@ -2253,11 +2259,11 @@
         <v/>
       </c>
       <c r="M45" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (45, 4,6)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (45, 3,6)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2281,7 +2287,7 @@
         <v>2</v>
       </c>
       <c r="I46" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (46,2,2,1)</v>
       </c>
       <c r="J46" t="str">
@@ -2294,15 +2300,15 @@
       </c>
       <c r="L46" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (46, 3,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (46, 2,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M46" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (46, 4,3)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (46, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N46" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (46, 5,2)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (46, 4,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -2325,7 +2331,7 @@
         <v>3</v>
       </c>
       <c r="I47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (47,3,2,1)</v>
       </c>
       <c r="J47" t="str">
@@ -2334,19 +2340,19 @@
       </c>
       <c r="K47" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (47, 2,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (47, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L47" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (47, 3,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (47, 2,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N47" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (47, 5,3)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (47, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
@@ -2363,12 +2369,12 @@
         <v>6</v>
       </c>
       <c r="I48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (48,1,2,3)</v>
       </c>
       <c r="J48" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (48, 1,6)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (48, 0,6)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K48" t="str">
         <f t="shared" si="1"/>
@@ -2379,11 +2385,11 @@
         <v/>
       </c>
       <c r="M48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2407,7 +2413,7 @@
         <v>2</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (49,4,2,1)</v>
       </c>
       <c r="J49" t="str">
@@ -2416,18 +2422,18 @@
       </c>
       <c r="K49" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (49, 2,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (49, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L49" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (49, 3,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (49, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M49" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (49, 4,2)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (49, 3,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N49" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2445,7 +2451,7 @@
         <v>5</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (50,3,2,2)</v>
       </c>
       <c r="J50" t="str">
@@ -2461,12 +2467,12 @@
         <v/>
       </c>
       <c r="M50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N50" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (50, 5,5)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (50, 4,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
@@ -2489,28 +2495,28 @@
         <v>3</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (51,2,2,1)</v>
       </c>
       <c r="J51" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (51, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (51, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K51" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (51, 2,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (51, 1,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L51" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M51" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N51" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (51, 5,3)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (51, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
@@ -2527,7 +2533,7 @@
         <v>5</v>
       </c>
       <c r="I52" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (52,4,2,2)</v>
       </c>
       <c r="J52" t="str">
@@ -2543,11 +2549,11 @@
         <v/>
       </c>
       <c r="M52" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (52, 4,5)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (52, 3,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2571,12 +2577,12 @@
         <v>2</v>
       </c>
       <c r="I53" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (53,1,2,1)</v>
       </c>
       <c r="J53" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (53, 1,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (53, 0,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K53" t="str">
         <f t="shared" si="1"/>
@@ -2584,15 +2590,15 @@
       </c>
       <c r="L53" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (53, 3,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (53, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M53" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N53" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (53, 5,2)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (53, 4,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
@@ -2609,7 +2615,7 @@
         <v>5</v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (54,1,2,2)</v>
       </c>
       <c r="J54" t="str">
@@ -2622,14 +2628,14 @@
       </c>
       <c r="L54" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (54, 3,5)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (54, 2,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M54" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2653,7 +2659,7 @@
         <v>3</v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (55,3,2,1)</v>
       </c>
       <c r="J55" t="str">
@@ -2662,19 +2668,19 @@
       </c>
       <c r="K55" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (55, 2,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (55, 1,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L55" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M55" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (55, 4,2)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (55, 3,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N55" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (55, 5,3)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (55, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
@@ -2694,7 +2700,7 @@
         <v>5</v>
       </c>
       <c r="I56" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (56,4,2,2)</v>
       </c>
       <c r="J56" t="str">
@@ -2710,12 +2716,12 @@
         <v/>
       </c>
       <c r="M56" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (56, 4,3)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (56, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N56" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (56, 5,5)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (56, 4,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
@@ -2738,27 +2744,27 @@
         <v>1</v>
       </c>
       <c r="I57" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (57,3,2,2)</v>
       </c>
       <c r="J57" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (57, 1,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (57, 0,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K57" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (57, 2,4)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (57, 1,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L57" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M57" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (57, 4,1)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (57, 3,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N57" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2782,7 +2788,7 @@
         <v>1</v>
       </c>
       <c r="I58" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (58,1,2,2)</v>
       </c>
       <c r="J58" t="str">
@@ -2791,19 +2797,19 @@
       </c>
       <c r="K58" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (58, 2,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (58, 1,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L58" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M58" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (58, 4,4)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (58, 3,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N58" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (58, 5,1)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (58, 4,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
@@ -2823,12 +2829,12 @@
         <v>3</v>
       </c>
       <c r="I59" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (59,5,2,2)</v>
       </c>
       <c r="J59" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (59, 1,5)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (59, 0,5)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K59" t="str">
         <f t="shared" si="1"/>
@@ -2836,14 +2842,14 @@
       </c>
       <c r="L59" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (59, 3,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (59, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M59" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N59" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2861,7 +2867,7 @@
         <v>6</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (60,2,2,3)</v>
       </c>
       <c r="J60" t="str">
@@ -2870,18 +2876,18 @@
       </c>
       <c r="K60" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (60, 2,6)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (60, 1,6)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L60" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M60" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N60" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2899,7 +2905,7 @@
         <v>6</v>
       </c>
       <c r="I61" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (61,3,2,3)</v>
       </c>
       <c r="J61" t="str">
@@ -2912,14 +2918,14 @@
       </c>
       <c r="L61" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (61, 3,6)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (61, 2,6)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M61" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N61" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2948,22 +2954,22 @@
       </c>
       <c r="J62" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (62, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (62, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K62" t="str">
         <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (62, 2,1)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (62, 1,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L62" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (62, 3,1)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (62, 2,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M62" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N62" t="str">
-        <f>IF(NOT(ISBLANK(H62)),"insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(H62)-3&amp;","&amp;H62&amp;")","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2981,12 +2987,12 @@
         <v>3</v>
       </c>
       <c r="I63" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (63,2,1,0)</v>
       </c>
       <c r="J63" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (63, 1,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (63, 0,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K63" t="str">
         <f t="shared" si="1"/>
@@ -2997,11 +3003,11 @@
         <v/>
       </c>
       <c r="M63" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -3025,12 +3031,12 @@
         <v>1</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (64,1,1,0)</v>
       </c>
       <c r="J64" t="str">
         <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (64, 1,1)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (64, 0,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K64" t="str">
         <f t="shared" si="1"/>
@@ -3038,15 +3044,15 @@
       </c>
       <c r="L64" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (64, 3,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (64, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M64" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N64" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (64, 5,1)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (64, 4,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -3069,7 +3075,7 @@
         <v>3</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (65,5,1,0)</v>
       </c>
       <c r="J65" t="str">
@@ -3082,15 +3088,15 @@
       </c>
       <c r="L65" t="str">
         <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (65, 3,1)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (65, 2,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M65" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (65, 4,1)</v>
+        <f t="shared" si="3"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (65, 3,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N65" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (65, 5,3)</v>
+        <f t="shared" si="4"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (65, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
@@ -3116,28 +3122,28 @@
         <v>1</v>
       </c>
       <c r="I66" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (66,4,1,0)</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (66, 1,2)</v>
+        <f t="shared" ref="J66:J101" si="7">IF(NOT(ISBLANK(D66)),"sql = ""insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(D66)-4&amp;","&amp;D66&amp;")""; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();","")</f>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (66, 0,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K66" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (66, 2,1)</v>
+        <f t="shared" ref="K66:K101" si="8">IF(NOT(ISBLANK(E66)),"sql = ""insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(E66)-4&amp;","&amp;E66&amp;")""; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();","")</f>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (66, 1,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L66" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (66, 3,1)</v>
+        <f t="shared" ref="L66:L101" si="9">IF(NOT(ISBLANK(F66)),"sql = ""insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(F66)-4&amp;","&amp;F66&amp;")""; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();","")</f>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (66, 2,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M66" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="M66:M101" si="10">IF(NOT(ISBLANK(G66)),"sql = ""insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(G66)-4&amp;","&amp;G66&amp;")""; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();","")</f>
         <v/>
       </c>
       <c r="N66" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (66, 5,1)</v>
+        <f t="shared" ref="N66:N101" si="11">IF(NOT(ISBLANK(H66)),"sql = ""insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(H66)-4&amp;","&amp;H66&amp;")""; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();","")</f>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (66, 4,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -3157,27 +3163,27 @@
         <v>1</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (67,5,1,0)</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" ref="J67:J101" si="6">IF(NOT(ISBLANK(D67)),"insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(D67)-3&amp;","&amp;D67&amp;")","")</f>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (67, 1,2)</v>
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (67, 0,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" ref="K67:K101" si="7">IF(NOT(ISBLANK(E67)),"insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(E67)-3&amp;","&amp;E67&amp;")","")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="L67" t="str">
-        <f t="shared" ref="L67:M101" si="8">IF(NOT(ISBLANK(F67)),"insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(F67)-3&amp;","&amp;F67&amp;")","")</f>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (67, 3,1)</v>
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (67, 2,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M67" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N67" t="str">
-        <f t="shared" ref="N67:N101" si="9">IF(NOT(ISBLANK(H67)),"insert into cost(fkCard, fkRessource, nbRessource) values ("&amp;ROW()&amp;", "&amp;COLUMN(H67)-3&amp;","&amp;H67&amp;")","")</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3198,27 +3204,27 @@
         <v>2</v>
       </c>
       <c r="I68" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (68,5,1,0)</v>
       </c>
       <c r="J68" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K68" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="L68" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (68, 3,2)</v>
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (68, 2,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M68" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (68, 4,2)</v>
+        <f t="shared" si="10"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (68, 3,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N68" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3236,27 +3242,27 @@
         <v>3</v>
       </c>
       <c r="I69" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (69,5,1,0)</v>
       </c>
       <c r="J69" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K69" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="L69" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M69" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (69, 4,3)</v>
+        <f t="shared" si="10"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (69, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N69" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3283,27 +3289,27 @@
         <v>1</v>
       </c>
       <c r="I70" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (70,5,1,0)</v>
       </c>
       <c r="J70" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (70, 1,1)</v>
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (70, 0,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K70" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (70, 2,2)</v>
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (70, 1,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L70" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (70, 3,1)</v>
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (70, 2,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M70" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (70, 4,1)</v>
+        <f t="shared" si="10"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (70, 3,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N70" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3327,27 +3333,27 @@
         <v>2</v>
       </c>
       <c r="I71" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (71,5,1,0)</v>
       </c>
       <c r="J71" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K71" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (71, 2,2)</v>
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (71, 1,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L71" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (71, 3,1)</v>
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (71, 2,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M71" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (71, 4,2)</v>
+        <f t="shared" si="10"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (71, 3,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N71" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3374,27 +3380,27 @@
         <v>1</v>
       </c>
       <c r="I72" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (72,5,1,0)</v>
       </c>
       <c r="J72" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (72, 1,1)</v>
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (72, 0,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K72" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (72, 2,1)</v>
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (72, 1,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L72" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (72, 3,1)</v>
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (72, 2,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M72" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (72, 4,1)</v>
+        <f t="shared" si="10"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (72, 3,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N72" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3412,27 +3418,27 @@
         <v>4</v>
       </c>
       <c r="I73" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (73,5,1,1)</v>
       </c>
       <c r="J73" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K73" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (73, 2,4)</v>
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (73, 1,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L73" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M73" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N73" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3459,28 +3465,28 @@
         <v>2</v>
       </c>
       <c r="I74" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (74,1,1,0)</v>
       </c>
       <c r="J74" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K74" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (74, 2,1)</v>
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (74, 1,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L74" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (74, 3,1)</v>
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (74, 2,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="M74" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (74, 4,1)</v>
+        <f t="shared" si="10"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (74, 3,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N74" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (74, 5,2)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (74, 4,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
@@ -3497,28 +3503,28 @@
         <v>3</v>
       </c>
       <c r="I75" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (75,1,1,0)</v>
       </c>
       <c r="J75" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K75" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="L75" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M75" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N75" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (75, 5,3)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (75, 4,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -3538,28 +3544,28 @@
         <v>2</v>
       </c>
       <c r="I76" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (76,1,1,0)</v>
       </c>
       <c r="J76" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (76, 1,2)</v>
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (76, 0,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="K76" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="L76" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M76" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N76" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (76, 5,2)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (76, 4,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
@@ -3579,27 +3585,27 @@
         <v>2</v>
       </c>
       <c r="I77" t="str">
-        <f t="shared" ref="I77:I101" si="10">"insert into card(idcard, fkRessource, level, nbPtPrestige) values (" &amp; ROW() &amp;"," &amp; B77 &amp; "," &amp; A77 &amp; "," &amp; C77 &amp; ")"</f>
+        <f t="shared" ref="I77:I101" si="12">"insert into card(idcard, fkRessource, level, nbPtPrestige) values (" &amp; ROW() &amp;"," &amp; B77 &amp; "," &amp; A77 &amp; "," &amp; C77 &amp; ")"</f>
         <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (77,1,1,0)</v>
       </c>
       <c r="J77" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K77" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (77, 2,1)</v>
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (77, 1,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="L77" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M77" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (77, 4,2)</v>
+        <f t="shared" si="10"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (77, 3,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3623,28 +3629,28 @@
         <v>2</v>
       </c>
       <c r="I78" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (78,1,1,0)</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K78" t="str">
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (78, 1,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="L78" t="str">
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (78, 2,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="M78" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (78,1,1,0)</v>
-      </c>
-      <c r="J78" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K78" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (78, 2,1)</v>
-      </c>
-      <c r="L78" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (78, 3,2)</v>
-      </c>
-      <c r="M78" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N78" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (78, 5,2)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (78, 4,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
@@ -3670,28 +3676,28 @@
         <v>1</v>
       </c>
       <c r="I79" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (79,1,1,0)</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K79" t="str">
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (79, 1,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="L79" t="str">
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (79, 2,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="M79" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (79,1,1,0)</v>
-      </c>
-      <c r="J79" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K79" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (79, 2,1)</v>
-      </c>
-      <c r="L79" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (79, 3,1)</v>
-      </c>
-      <c r="M79" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (79, 4,1)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (79, 3,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N79" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (79, 5,1)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (79, 4,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -3708,28 +3714,28 @@
         <v>4</v>
       </c>
       <c r="I80" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (80,1,1,1)</v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K80" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M80" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (80,1,1,1)</v>
-      </c>
-      <c r="J80" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K80" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L80" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M80" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N80" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (80, 5,4)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (80, 4,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
@@ -3752,28 +3758,28 @@
         <v>2</v>
       </c>
       <c r="I81" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (81,3,1,0)</v>
+      </c>
+      <c r="J81" t="str">
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (81, 0,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="K81" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L81" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M81" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (81,3,1,0)</v>
-      </c>
-      <c r="J81" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (81, 1,1)</v>
-      </c>
-      <c r="K81" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L81" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M81" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (81, 4,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (81, 3,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N81" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (81, 5,2)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (81, 4,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
@@ -3793,28 +3799,28 @@
         <v>2</v>
       </c>
       <c r="I82" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (82,3,1,0)</v>
+      </c>
+      <c r="J82" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K82" t="str">
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (82, 1,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="L82" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M82" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (82,3,1,0)</v>
-      </c>
-      <c r="J82" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K82" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (82, 2,2)</v>
-      </c>
-      <c r="L82" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M82" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N82" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (82, 5,2)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (82, 4,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
@@ -3831,27 +3837,27 @@
         <v>3</v>
       </c>
       <c r="I83" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (83,3,1,0)</v>
+      </c>
+      <c r="J83" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K83" t="str">
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (83, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="L83" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M83" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (83,3,1,0)</v>
-      </c>
-      <c r="J83" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K83" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (83, 2,3)</v>
-      </c>
-      <c r="L83" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M83" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N83" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3872,27 +3878,27 @@
         <v>2</v>
       </c>
       <c r="I84" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (84,3,1,0)</v>
+      </c>
+      <c r="J84" t="str">
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (84, 0,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="K84" t="str">
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (84, 1,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="L84" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M84" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (84,3,1,0)</v>
-      </c>
-      <c r="J84" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (84, 1,1)</v>
-      </c>
-      <c r="K84" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (84, 2,2)</v>
-      </c>
-      <c r="L84" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M84" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N84" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3919,28 +3925,28 @@
         <v>1</v>
       </c>
       <c r="I85" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (85,3,1,0)</v>
+      </c>
+      <c r="J85" t="str">
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (85, 0,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="K85" t="str">
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (85, 1,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="L85" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M85" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (85,3,1,0)</v>
-      </c>
-      <c r="J85" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (85, 1,1)</v>
-      </c>
-      <c r="K85" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (85, 2,1)</v>
-      </c>
-      <c r="L85" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M85" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (85, 4,1)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (85, 3,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N85" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (85, 5,1)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (85, 4,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -3966,28 +3972,28 @@
         <v>1</v>
       </c>
       <c r="I86" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (86,3,1,0)</v>
+      </c>
+      <c r="J86" t="str">
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (86, 0,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="K86" t="str">
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (86, 1,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="L86" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M86" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (86,3,1,0)</v>
-      </c>
-      <c r="J86" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (86, 1,1)</v>
-      </c>
-      <c r="K86" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (86, 2,1)</v>
-      </c>
-      <c r="L86" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M86" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (86, 4,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (86, 3,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N86" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (86, 5,1)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (86, 4,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
@@ -4004,27 +4010,27 @@
         <v>4</v>
       </c>
       <c r="I87" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (87,3,1,1)</v>
+      </c>
+      <c r="J87" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K87" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L87" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M87" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (87,3,1,1)</v>
-      </c>
-      <c r="J87" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K87" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L87" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M87" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (87, 4,4)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (87, 3,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N87" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -4051,28 +4057,28 @@
         <v>1</v>
       </c>
       <c r="I88" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (88,4,1,0)</v>
+      </c>
+      <c r="J88" t="str">
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (88, 0,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="K88" t="str">
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (88, 1,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="L88" t="str">
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (88, 2,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="M88" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (88,4,1,0)</v>
-      </c>
-      <c r="J88" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (88, 1,1)</v>
-      </c>
-      <c r="K88" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (88, 2,1)</v>
-      </c>
-      <c r="L88" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (88, 3,1)</v>
-      </c>
-      <c r="M88" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N88" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (88, 5,1)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (88, 4,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
@@ -4092,28 +4098,28 @@
         <v>1</v>
       </c>
       <c r="I89" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (89,4,1,0)</v>
+      </c>
+      <c r="J89" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K89" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L89" t="str">
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (89, 2,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="M89" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (89,4,1,0)</v>
-      </c>
-      <c r="J89" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K89" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L89" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (89, 3,2)</v>
-      </c>
-      <c r="M89" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N89" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (89, 5,1)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (89, 4,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
@@ -4130,27 +4136,27 @@
         <v>3</v>
       </c>
       <c r="I90" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (90,4,1,0)</v>
+      </c>
+      <c r="J90" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K90" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L90" t="str">
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (90, 2,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="M90" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (90,4,1,0)</v>
-      </c>
-      <c r="J90" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K90" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L90" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (90, 3,3)</v>
-      </c>
-      <c r="M90" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N90" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -4174,28 +4180,28 @@
         <v>1</v>
       </c>
       <c r="I91" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (91,4,1,0)</v>
+      </c>
+      <c r="J91" t="str">
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (91, 0,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="K91" t="str">
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (91, 1,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="L91" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M91" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (91,4,1,0)</v>
-      </c>
-      <c r="J91" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (91, 1,2)</v>
-      </c>
-      <c r="K91" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (91, 2,2)</v>
-      </c>
-      <c r="L91" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M91" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N91" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (91, 5,1)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (91, 4,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
@@ -4215,27 +4221,27 @@
         <v>2</v>
       </c>
       <c r="I92" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (92,4,1,0)</v>
+      </c>
+      <c r="J92" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K92" t="str">
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (92, 1,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="L92" t="str">
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (92, 2,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="M92" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (92,4,1,0)</v>
-      </c>
-      <c r="J92" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K92" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (92, 2,2)</v>
-      </c>
-      <c r="L92" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (92, 3,2)</v>
-      </c>
-      <c r="M92" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N92" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -4259,27 +4265,27 @@
         <v>1</v>
       </c>
       <c r="I93" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (93,4,1,0)</v>
+      </c>
+      <c r="J93" t="str">
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (93, 0,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="K93" t="str">
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (93, 1,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="L93" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M93" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (93,4,1,0)</v>
-      </c>
-      <c r="J93" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (93, 1,1)</v>
-      </c>
-      <c r="K93" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (93, 2,3)</v>
-      </c>
-      <c r="L93" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M93" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (93, 4,1)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (93, 3,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N93" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -4297,27 +4303,27 @@
         <v>4</v>
       </c>
       <c r="I94" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (94,4,1,1)</v>
+      </c>
+      <c r="J94" t="str">
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (94, 0,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="K94" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L94" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M94" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (94,4,1,1)</v>
-      </c>
-      <c r="J94" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (94, 1,4)</v>
-      </c>
-      <c r="K94" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L94" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M94" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N94" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -4341,28 +4347,28 @@
         <v>1</v>
       </c>
       <c r="I95" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (95,2,1,0)</v>
+      </c>
+      <c r="J95" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K95" t="str">
+        <f t="shared" si="8"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (95, 1,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="L95" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M95" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (95,2,1,0)</v>
-      </c>
-      <c r="J95" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K95" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (95, 2,1)</v>
-      </c>
-      <c r="L95" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M95" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (95, 4,3)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (95, 3,3)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N95" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (95, 5,1)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (95, 4,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
@@ -4385,27 +4391,27 @@
         <v>1</v>
       </c>
       <c r="I96" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (96,2,1,0)</v>
+      </c>
+      <c r="J96" t="str">
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (96, 0,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="K96" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L96" t="str">
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (96, 2,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="M96" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (96,2,1,0)</v>
-      </c>
-      <c r="J96" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (96, 1,2)</v>
-      </c>
-      <c r="K96" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L96" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (96, 3,2)</v>
-      </c>
-      <c r="M96" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (96, 4,1)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (96, 3,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N96" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -4432,28 +4438,28 @@
         <v>1</v>
       </c>
       <c r="I97" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (97,2,1,0)</v>
+      </c>
+      <c r="J97" t="str">
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (97, 0,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="K97" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L97" t="str">
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (97, 2,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="M97" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (97,2,1,0)</v>
-      </c>
-      <c r="J97" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (97, 1,1)</v>
-      </c>
-      <c r="K97" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L97" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (97, 3,1)</v>
-      </c>
-      <c r="M97" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (97, 4,1)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (97, 3,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N97" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (97, 5,1)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (97, 4,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
@@ -4473,27 +4479,27 @@
         <v>2</v>
       </c>
       <c r="I98" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (98,2,1,0)</v>
+      </c>
+      <c r="J98" t="str">
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (98, 0,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="K98" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L98" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M98" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (98,2,1,0)</v>
-      </c>
-      <c r="J98" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (98, 1,2)</v>
-      </c>
-      <c r="K98" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L98" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M98" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (98, 4,2)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (98, 3,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N98" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -4514,28 +4520,28 @@
         <v>2</v>
       </c>
       <c r="I99" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (99,2,1,0)</v>
+      </c>
+      <c r="J99" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K99" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L99" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M99" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (99,2,1,0)</v>
-      </c>
-      <c r="J99" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K99" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L99" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M99" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (99, 4,1)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (99, 3,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N99" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (99, 5,2)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (99, 4,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
@@ -4561,28 +4567,28 @@
         <v>1</v>
       </c>
       <c r="I100" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (100,2,1,0)</v>
+      </c>
+      <c r="J100" t="str">
+        <f t="shared" si="7"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (100, 0,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="K100" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L100" t="str">
+        <f t="shared" si="9"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (100, 2,2)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+      </c>
+      <c r="M100" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (100,2,1,0)</v>
-      </c>
-      <c r="J100" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (100, 1,1)</v>
-      </c>
-      <c r="K100" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L100" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (100, 3,2)</v>
-      </c>
-      <c r="M100" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (100, 4,1)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (100, 3,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N100" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (100, 5,1)</v>
+        <f t="shared" si="11"/>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (100, 4,1)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
@@ -4599,27 +4605,27 @@
         <v>4</v>
       </c>
       <c r="I101" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (101,2,1,1)</v>
+      </c>
+      <c r="J101" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K101" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L101" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M101" t="str">
         <f t="shared" si="10"/>
-        <v>insert into card(idcard, fkRessource, level, nbPtPrestige) values (101,2,1,1)</v>
-      </c>
-      <c r="J101" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K101" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L101" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="M101" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into cost(fkCard, fkRessource, nbRessource) values (101, 4,4)</v>
+        <v>sql = "insert into cost(fkCard, fkRessource, nbRessource) values (101, 3,4)"; command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
       <c r="N101" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>

</xml_diff>